<commit_message>
24hr change and trend fixed
</commit_message>
<xml_diff>
--- a/classes+unitTests/stockAnalysis/Book2.xlsx
+++ b/classes+unitTests/stockAnalysis/Book2.xlsx
@@ -8,17 +8,28 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zimul\Documents\python\classes+unitTests\stockAnalysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C576136-3AE9-4196-96C2-27D1846F9E56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7B6C04E-F445-45E0-9F31-96BCD0B2C101}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -367,7 +378,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -415,7 +426,7 @@
         <v>6</v>
       </c>
       <c r="D3">
-        <v>110</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -471,7 +482,7 @@
         <v>6</v>
       </c>
       <c r="D7">
-        <v>50</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -485,7 +496,7 @@
         <v>6</v>
       </c>
       <c r="D8">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -499,7 +510,7 @@
         <v>6</v>
       </c>
       <c r="D9">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
minor touches before ui
</commit_message>
<xml_diff>
--- a/classes+unitTests/stockAnalysis/Book2.xlsx
+++ b/classes+unitTests/stockAnalysis/Book2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zimul\Documents\python\classes+unitTests\stockAnalysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7B6C04E-F445-45E0-9F31-96BCD0B2C101}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD654670-C2C5-46E7-A8D5-54FA1B643FF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="11">
   <si>
     <t>Symbol</t>
   </si>
@@ -57,6 +57,18 @@
   </si>
   <si>
     <t>dk</t>
+  </si>
+  <si>
+    <t>ms</t>
+  </si>
+  <si>
+    <t>us</t>
+  </si>
+  <si>
+    <t>ch</t>
+  </si>
+  <si>
+    <t>nz</t>
   </si>
 </sst>
 </file>
@@ -375,10 +387,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="A14" sqref="A14:XFD14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -412,7 +424,7 @@
         <v>6</v>
       </c>
       <c r="D2">
-        <v>100</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -426,7 +438,7 @@
         <v>6</v>
       </c>
       <c r="D3">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -440,7 +452,7 @@
         <v>6</v>
       </c>
       <c r="D4">
-        <v>100</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -454,7 +466,7 @@
         <v>6</v>
       </c>
       <c r="D5">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -468,7 +480,7 @@
         <v>6</v>
       </c>
       <c r="D6">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -482,7 +494,7 @@
         <v>6</v>
       </c>
       <c r="D7">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -496,7 +508,7 @@
         <v>6</v>
       </c>
       <c r="D8">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -510,7 +522,63 @@
         <v>6</v>
       </c>
       <c r="D9">
-        <v>40</v>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="1">
+        <v>41244</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="1">
+        <v>41245</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="1">
+        <v>41246</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="1">
+        <v>41247</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
basic risk analysis added
</commit_message>
<xml_diff>
--- a/classes+unitTests/stockAnalysis/Book2.xlsx
+++ b/classes+unitTests/stockAnalysis/Book2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zimul\Documents\python\classes+unitTests\stockAnalysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD654670-C2C5-46E7-A8D5-54FA1B643FF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0519C9B0-C0CB-4B9E-B2FD-45F59BE835E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4725" yWindow="225" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -390,7 +390,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:XFD14"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -466,7 +466,7 @@
         <v>6</v>
       </c>
       <c r="D5">
-        <v>85</v>
+        <v>500</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>